<commit_message>
BALP 1.1.1 and history file updates
</commit_message>
<xml_diff>
--- a/ITI/BALP/CodeSystem-AuthZsubType.xlsx
+++ b/ITI/BALP/CodeSystem-AuthZsubType.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>1.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,10 +54,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-04T10:16:52-05:00</t>
+    <t>2022-10-21T09:04:31-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -343,128 +346,130 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -482,39 +487,39 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2"/>
     </row>

</xml_diff>